<commit_message>
add export loop flow contrast report
</commit_message>
<xml_diff>
--- a/CBMWebApi/wwwroot/ExcelTempate/计量支路流量对比报告.xlsx
+++ b/CBMWebApi/wwwroot/ExcelTempate/计量支路流量对比报告.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wwwroot\WCBMWebApi\CBMWebApi\wwwroot\ExcelTempate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F293552B-90B4-44C0-95F8-9623AE01E266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8768E46-7C91-4BB1-8B26-A1F052EB3648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -690,7 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -708,21 +708,61 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
@@ -731,48 +771,6 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
@@ -789,8 +787,13 @@
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1087,68 +1090,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8"/>
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14"/>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8"/>
+      <c r="E2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8"/>
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8"/>
+      <c r="E3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="17" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1192,79 +1195,79 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8"/>
+      <c r="B8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14"/>
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8"/>
+      <c r="E8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="8"/>
+      <c r="B9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8"/>
+      <c r="E9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="16" t="s">
+      <c r="D11" s="30"/>
+      <c r="E11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="30"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1310,124 +1313,124 @@
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8"/>
+      <c r="B16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8"/>
+      <c r="E16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8"/>
+      <c r="B17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="14"/>
       <c r="D17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="8"/>
+      <c r="E17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="21"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="22" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="23"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="28"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:F13"/>
@@ -1438,16 +1441,16 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>